<commit_message>
sanitized data in year_state_observation and made choropleth plot
</commit_message>
<xml_diff>
--- a/year_state_observations.xlsx
+++ b/year_state_observations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emil\Desktop\UNI\DataVisualization\R_opgaver\Project\DataVis-2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kinky\Rstudio\DataVis-2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C08460D5-9B99-410A-8792-51B43797F79F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F260D0BD-432E-435F-B527-F34B83DB9306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2D0E99FB-9E44-419D-9F1A-6A34DA89E689}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2D0E99FB-9E44-419D-9F1A-6A34DA89E689}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -36,130 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
-  <si>
-    <t>Georgia</t>
-  </si>
-  <si>
-    <t>Hawaii</t>
-  </si>
-  <si>
-    <t>Idaho</t>
-  </si>
-  <si>
-    <t>Illinois</t>
-  </si>
-  <si>
-    <t>Indiana</t>
-  </si>
-  <si>
-    <t>Iowa</t>
-  </si>
-  <si>
-    <t>Kansas</t>
-  </si>
-  <si>
-    <t>Kentucky</t>
-  </si>
-  <si>
-    <t>Louisiana</t>
-  </si>
-  <si>
-    <t>Maine</t>
-  </si>
-  <si>
-    <t>Maryland</t>
-  </si>
-  <si>
-    <t>Massachusetts</t>
-  </si>
-  <si>
-    <t>Michigan</t>
-  </si>
-  <si>
-    <t>Minnesota</t>
-  </si>
-  <si>
-    <t>Mississippi</t>
-  </si>
-  <si>
-    <t>Missouri</t>
-  </si>
-  <si>
-    <t>Montana</t>
-  </si>
-  <si>
-    <t>Nebraska</t>
-  </si>
-  <si>
-    <t>Nevada</t>
-  </si>
-  <si>
-    <t>New Hampshire</t>
-  </si>
-  <si>
-    <t>New Jersey</t>
-  </si>
-  <si>
-    <t>New Mexico</t>
-  </si>
-  <si>
-    <t>New York</t>
-  </si>
-  <si>
-    <t>North Carolina</t>
-  </si>
-  <si>
-    <t>North Dakota</t>
-  </si>
-  <si>
-    <t>Ohio</t>
-  </si>
-  <si>
-    <t>Oklahoma</t>
-  </si>
-  <si>
-    <t>Oregon</t>
-  </si>
-  <si>
-    <t>Pennsylvania</t>
-  </si>
-  <si>
-    <t>Rhode Island</t>
-  </si>
-  <si>
-    <t>South Carolina</t>
-  </si>
-  <si>
-    <t>South Dakota</t>
-  </si>
-  <si>
-    <t>Tennessee</t>
-  </si>
-  <si>
-    <t>Texas</t>
-  </si>
-  <si>
-    <t>Utah</t>
-  </si>
-  <si>
-    <t>Vermont</t>
-  </si>
-  <si>
-    <t>Virginia</t>
-  </si>
-  <si>
-    <t>Washington</t>
-  </si>
-  <si>
-    <t>West Virginia</t>
-  </si>
-  <si>
-    <t>Wisconsin</t>
-  </si>
-  <si>
-    <t>Wyoming</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>alabama</t>
   </si>
@@ -186,6 +63,135 @@
   </si>
   <si>
     <t>florida</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>population</t>
+  </si>
+  <si>
+    <t>georgia</t>
+  </si>
+  <si>
+    <t>hawaii</t>
+  </si>
+  <si>
+    <t>idaho</t>
+  </si>
+  <si>
+    <t>illinois</t>
+  </si>
+  <si>
+    <t>indiana</t>
+  </si>
+  <si>
+    <t>iowa</t>
+  </si>
+  <si>
+    <t>kansas</t>
+  </si>
+  <si>
+    <t>kentucky</t>
+  </si>
+  <si>
+    <t>maine</t>
+  </si>
+  <si>
+    <t>maryland</t>
+  </si>
+  <si>
+    <t>massachusetts</t>
+  </si>
+  <si>
+    <t>michigan</t>
+  </si>
+  <si>
+    <t>minnesota</t>
+  </si>
+  <si>
+    <t>mississippi</t>
+  </si>
+  <si>
+    <t>missouri</t>
+  </si>
+  <si>
+    <t>montana</t>
+  </si>
+  <si>
+    <t>nebraska</t>
+  </si>
+  <si>
+    <t>nevada</t>
+  </si>
+  <si>
+    <t>ohio</t>
+  </si>
+  <si>
+    <t>oklahoma</t>
+  </si>
+  <si>
+    <t>oregon</t>
+  </si>
+  <si>
+    <t>pennsylvania</t>
+  </si>
+  <si>
+    <t>tennessee</t>
+  </si>
+  <si>
+    <t>texas</t>
+  </si>
+  <si>
+    <t>utah</t>
+  </si>
+  <si>
+    <t>vermont</t>
+  </si>
+  <si>
+    <t>virginia</t>
+  </si>
+  <si>
+    <t>washington</t>
+  </si>
+  <si>
+    <t>wisconsin</t>
+  </si>
+  <si>
+    <t>wyoming</t>
+  </si>
+  <si>
+    <t>north carolina</t>
+  </si>
+  <si>
+    <t>north dakota</t>
+  </si>
+  <si>
+    <t>south carolina</t>
+  </si>
+  <si>
+    <t>south dakota</t>
+  </si>
+  <si>
+    <t>west virginia</t>
+  </si>
+  <si>
+    <t>new mexico</t>
+  </si>
+  <si>
+    <t>new york</t>
+  </si>
+  <si>
+    <t>rhode island</t>
+  </si>
+  <si>
+    <t>louisiana</t>
+  </si>
+  <si>
+    <t>new hampshire</t>
+  </si>
+  <si>
+    <t>new jersey</t>
   </si>
 </sst>
 </file>
@@ -230,12 +236,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -252,7 +261,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -548,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E0E4920-5424-4490-B76F-694BE8C4882F}">
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="102" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,339 +569,339 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
         <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2">
-        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>220</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>44</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>40</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>546</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>192</v>
+        <v>546</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>65</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>16</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>338</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>117</v>
+        <v>338</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B11">
-        <v>28</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B12">
-        <v>69</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B13">
-        <v>142</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B14">
-        <v>77</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B15">
-        <v>40</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B16">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B17">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B18">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="B19">
-        <v>67</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B20">
-        <v>98</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B21">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B22">
-        <v>131</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B23">
-        <v>77</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B24">
-        <v>31</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B25">
-        <v>109</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B26">
-        <v>45</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B27">
-        <v>16</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B28">
-        <v>61</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B29">
-        <v>50</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="B30">
-        <v>125</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="B31">
-        <v>73</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="B32">
-        <v>203</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="B33">
-        <v>211</v>
+        <v>203</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="B34">
-        <v>11</v>
+        <v>211</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="B35">
-        <v>141</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B36">
-        <v>43</v>
+        <v>141</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B37">
-        <v>157</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B38">
-        <v>189</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B39">
-        <v>29</v>
+        <v>189</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="B40">
-        <v>88</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="B41">
-        <v>20</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="B42">
-        <v>108</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -900,7 +909,7 @@
         <v>33</v>
       </c>
       <c r="B43">
-        <v>139</v>
+        <v>108</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -908,7 +917,7 @@
         <v>34</v>
       </c>
       <c r="B44">
-        <v>84</v>
+        <v>139</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -916,7 +925,7 @@
         <v>35</v>
       </c>
       <c r="B45">
-        <v>19</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -924,7 +933,7 @@
         <v>36</v>
       </c>
       <c r="B46">
-        <v>108</v>
+        <v>19</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -932,7 +941,7 @@
         <v>37</v>
       </c>
       <c r="B47">
-        <v>215</v>
+        <v>108</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -940,79 +949,88 @@
         <v>38</v>
       </c>
       <c r="B48">
-        <v>28</v>
+        <v>215</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B49">
-        <v>114</v>
+        <v>28</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B50">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B50">
+      <c r="B51">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="https://state.1keydata.com/alabama.php" xr:uid="{BA461CC7-AD6D-40DA-A6A2-9A6253BDE39C}"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://state.1keydata.com/alaska.php" xr:uid="{15150102-1D74-4D09-AD9D-7C16C13CF533}"/>
-    <hyperlink ref="A3" r:id="rId3" display="https://state.1keydata.com/arizona.php" xr:uid="{7FACD27A-D3CB-4C07-9AEF-3317326D285F}"/>
-    <hyperlink ref="A4" r:id="rId4" display="https://state.1keydata.com/arkansas.php" xr:uid="{FE00D17A-FEF6-4442-9D26-1D04E6DFF723}"/>
-    <hyperlink ref="A5" r:id="rId5" display="https://state.1keydata.com/california.php" xr:uid="{CB77828C-677B-4A4D-96BF-25A734B1E9E7}"/>
-    <hyperlink ref="A6" r:id="rId6" display="https://state.1keydata.com/colorado.php" xr:uid="{19FFB7E7-7462-45EE-B568-76A92184DFAE}"/>
-    <hyperlink ref="A7" r:id="rId7" display="https://state.1keydata.com/connecticut.php" xr:uid="{12FCB216-CC65-4A3B-B570-2EE93083E1D3}"/>
-    <hyperlink ref="A8" r:id="rId8" display="https://state.1keydata.com/delaware.php" xr:uid="{87E572C5-12FC-456E-8629-C51A34DD7D0A}"/>
-    <hyperlink ref="A9" r:id="rId9" display="https://state.1keydata.com/florida.php" xr:uid="{3779ECEA-C9D7-4D5E-B167-CED756F3BA10}"/>
-    <hyperlink ref="A10" r:id="rId10" display="https://state.1keydata.com/georgia.php" xr:uid="{1E7D53D7-3DFD-4BEA-A42D-0957C468BA12}"/>
-    <hyperlink ref="A11" r:id="rId11" display="https://state.1keydata.com/hawaii.php" xr:uid="{87C5BF53-98B4-4FD2-8CCD-2C91015F63A1}"/>
-    <hyperlink ref="A12" r:id="rId12" display="https://state.1keydata.com/idaho.php" xr:uid="{4EFCEF69-EE30-43D0-A047-019D17EE8C55}"/>
-    <hyperlink ref="A13" r:id="rId13" display="https://state.1keydata.com/illinois.php" xr:uid="{702E882F-D9B5-46D8-B4A6-8129CEDE9AC3}"/>
-    <hyperlink ref="A14" r:id="rId14" display="https://state.1keydata.com/indiana.php" xr:uid="{6009634B-6795-4710-8276-0180FB6733B5}"/>
-    <hyperlink ref="A15" r:id="rId15" display="https://state.1keydata.com/iowa.php" xr:uid="{76802265-CEB5-470A-A1E7-51C4D8A9EFBF}"/>
-    <hyperlink ref="A16" r:id="rId16" display="https://state.1keydata.com/kansas.php" xr:uid="{DAB489D2-D8C2-4493-8DB9-D933617BCE4D}"/>
-    <hyperlink ref="A17" r:id="rId17" display="https://state.1keydata.com/kentucky.php" xr:uid="{BB8E9FEE-C1FC-436C-B81B-F99F3CF33F79}"/>
-    <hyperlink ref="A18" r:id="rId18" display="https://state.1keydata.com/louisiana.php" xr:uid="{47CD2271-F57A-4C93-8B8A-E175F9DC25D3}"/>
-    <hyperlink ref="A19" r:id="rId19" display="https://state.1keydata.com/maine.php" xr:uid="{696FE484-AF5D-4275-BEAC-CA2A9B91E306}"/>
-    <hyperlink ref="A20" r:id="rId20" display="https://state.1keydata.com/maryland.php" xr:uid="{848C9F60-1B78-4728-B3B2-11F5FDBAF18B}"/>
-    <hyperlink ref="A21" r:id="rId21" display="https://state.1keydata.com/massachusetts.php" xr:uid="{65685229-3E48-4624-A514-AF998DC09814}"/>
-    <hyperlink ref="A22" r:id="rId22" display="https://state.1keydata.com/michigan.php" xr:uid="{3B6313F6-0A70-4F36-9A3F-A6F2D667817B}"/>
-    <hyperlink ref="A23" r:id="rId23" display="https://state.1keydata.com/minnesota.php" xr:uid="{53C2CC79-9C37-4E14-902D-2F1EBB3DC32D}"/>
-    <hyperlink ref="A24" r:id="rId24" display="https://state.1keydata.com/mississippi.php" xr:uid="{D243D5F7-C97C-4A86-9948-94AF122BD89E}"/>
-    <hyperlink ref="A25" r:id="rId25" display="https://state.1keydata.com/missouri.php" xr:uid="{A2801156-5393-4FF3-ACB5-DC74A4936F00}"/>
-    <hyperlink ref="A26" r:id="rId26" display="https://state.1keydata.com/montana.php" xr:uid="{4DDD9FB0-3AB6-47BE-84CA-33056B28C7F7}"/>
-    <hyperlink ref="A27" r:id="rId27" display="https://state.1keydata.com/nebraska.php" xr:uid="{B2ED209B-EFB1-492A-9277-E442426CBD4D}"/>
-    <hyperlink ref="A28" r:id="rId28" display="https://state.1keydata.com/nevada.php" xr:uid="{C2B6E048-65E5-41D0-871D-151EC25EAFA9}"/>
-    <hyperlink ref="A29" r:id="rId29" display="https://state.1keydata.com/new-hampshire.php" xr:uid="{F3577E82-C6D7-4532-86BB-325E0F092D04}"/>
-    <hyperlink ref="A30" r:id="rId30" display="https://state.1keydata.com/new-jersey.php" xr:uid="{C5BE69F9-14E0-4D01-B38D-14E74273A248}"/>
-    <hyperlink ref="A31" r:id="rId31" display="https://state.1keydata.com/new-mexico.php" xr:uid="{C74BEB2A-EDCF-4AAB-8B12-25FF38DDFC30}"/>
-    <hyperlink ref="A32" r:id="rId32" display="https://state.1keydata.com/new-york.php" xr:uid="{DAA1D700-972B-4EA1-99C3-2C843EADE48B}"/>
-    <hyperlink ref="A33" r:id="rId33" display="https://state.1keydata.com/north-carolina.php" xr:uid="{90E79B03-7106-4FF1-A746-14D3D3A39497}"/>
-    <hyperlink ref="A34" r:id="rId34" display="https://state.1keydata.com/north-dakota.php" xr:uid="{A5D2581E-1FBD-4DF9-A15D-F570D6B09EDF}"/>
-    <hyperlink ref="A35" r:id="rId35" display="https://state.1keydata.com/ohio.php" xr:uid="{A9AFF7C4-41AB-4BAA-AE07-DC79AD68A17C}"/>
-    <hyperlink ref="A36" r:id="rId36" display="https://state.1keydata.com/oklahoma.php" xr:uid="{9405CCC4-606C-4856-ABE2-83B3F72F2186}"/>
-    <hyperlink ref="A37" r:id="rId37" display="https://state.1keydata.com/oregon.php" xr:uid="{9FB3B5AA-5334-4D12-90CD-130D956D6152}"/>
-    <hyperlink ref="A38" r:id="rId38" display="https://state.1keydata.com/pennsylvania.php" xr:uid="{52D4C6A8-D8D9-4096-B2B9-E55A2F3388E9}"/>
-    <hyperlink ref="A39" r:id="rId39" display="https://state.1keydata.com/rhode-island.php" xr:uid="{F0D395DD-C6D5-434F-AE51-AC19A46BB531}"/>
-    <hyperlink ref="A40" r:id="rId40" display="https://state.1keydata.com/south-carolina.php" xr:uid="{2EC88C7B-5678-4EC6-999E-00BF03F0A65B}"/>
-    <hyperlink ref="A41" r:id="rId41" display="https://state.1keydata.com/south-dakota.php" xr:uid="{F45830B5-E60D-4FE0-8498-E5EA018ADC4B}"/>
-    <hyperlink ref="A42" r:id="rId42" display="https://state.1keydata.com/tennessee.php" xr:uid="{3159AE8B-C86C-4D42-B8CA-81CD3040D913}"/>
-    <hyperlink ref="A43" r:id="rId43" display="https://state.1keydata.com/texas.php" xr:uid="{C644E441-99E1-43C3-AD93-46046DB2B920}"/>
-    <hyperlink ref="A44" r:id="rId44" display="https://state.1keydata.com/utah.php" xr:uid="{7951D014-7331-43DF-9227-6810FEF48140}"/>
-    <hyperlink ref="A45" r:id="rId45" display="https://state.1keydata.com/vermont.php" xr:uid="{F65F39C8-5EEB-47BC-927C-A71E472CE1CD}"/>
-    <hyperlink ref="A46" r:id="rId46" display="https://state.1keydata.com/virginia.php" xr:uid="{137664BF-CFED-4997-9C7B-B7CF5E84F63D}"/>
-    <hyperlink ref="A47" r:id="rId47" display="https://state.1keydata.com/washington.php" xr:uid="{270E5710-6AAF-409B-9993-F717B633AEB6}"/>
-    <hyperlink ref="A48" r:id="rId48" display="https://state.1keydata.com/west-virginia.php" xr:uid="{E1781213-0A6E-4777-ABEB-4EC3D1727395}"/>
-    <hyperlink ref="A49" r:id="rId49" display="https://state.1keydata.com/wisconsin.php" xr:uid="{E794A894-3E0F-41FA-9217-DB360B278E19}"/>
-    <hyperlink ref="A50" r:id="rId50" display="https://state.1keydata.com/wyoming.php" xr:uid="{9B0DB648-20AF-446A-BBDE-351804DAA998}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://state.1keydata.com/alabama.php" xr:uid="{BA461CC7-AD6D-40DA-A6A2-9A6253BDE39C}"/>
+    <hyperlink ref="A3" r:id="rId2" display="https://state.1keydata.com/alaska.php" xr:uid="{15150102-1D74-4D09-AD9D-7C16C13CF533}"/>
+    <hyperlink ref="A4" r:id="rId3" display="https://state.1keydata.com/arizona.php" xr:uid="{7FACD27A-D3CB-4C07-9AEF-3317326D285F}"/>
+    <hyperlink ref="A5" r:id="rId4" display="https://state.1keydata.com/arkansas.php" xr:uid="{FE00D17A-FEF6-4442-9D26-1D04E6DFF723}"/>
+    <hyperlink ref="A6" r:id="rId5" display="https://state.1keydata.com/california.php" xr:uid="{CB77828C-677B-4A4D-96BF-25A734B1E9E7}"/>
+    <hyperlink ref="A7" r:id="rId6" display="https://state.1keydata.com/colorado.php" xr:uid="{19FFB7E7-7462-45EE-B568-76A92184DFAE}"/>
+    <hyperlink ref="A8" r:id="rId7" display="https://state.1keydata.com/connecticut.php" xr:uid="{12FCB216-CC65-4A3B-B570-2EE93083E1D3}"/>
+    <hyperlink ref="A9" r:id="rId8" display="https://state.1keydata.com/delaware.php" xr:uid="{87E572C5-12FC-456E-8629-C51A34DD7D0A}"/>
+    <hyperlink ref="A10" r:id="rId9" display="https://state.1keydata.com/florida.php" xr:uid="{3779ECEA-C9D7-4D5E-B167-CED756F3BA10}"/>
+    <hyperlink ref="A11" r:id="rId10" display="https://state.1keydata.com/georgia.php" xr:uid="{1E7D53D7-3DFD-4BEA-A42D-0957C468BA12}"/>
+    <hyperlink ref="A12" r:id="rId11" display="https://state.1keydata.com/hawaii.php" xr:uid="{87C5BF53-98B4-4FD2-8CCD-2C91015F63A1}"/>
+    <hyperlink ref="A13" r:id="rId12" display="https://state.1keydata.com/idaho.php" xr:uid="{4EFCEF69-EE30-43D0-A047-019D17EE8C55}"/>
+    <hyperlink ref="A14" r:id="rId13" display="https://state.1keydata.com/illinois.php" xr:uid="{702E882F-D9B5-46D8-B4A6-8129CEDE9AC3}"/>
+    <hyperlink ref="A15" r:id="rId14" display="https://state.1keydata.com/indiana.php" xr:uid="{6009634B-6795-4710-8276-0180FB6733B5}"/>
+    <hyperlink ref="A16" r:id="rId15" display="https://state.1keydata.com/iowa.php" xr:uid="{76802265-CEB5-470A-A1E7-51C4D8A9EFBF}"/>
+    <hyperlink ref="A17" r:id="rId16" display="https://state.1keydata.com/kansas.php" xr:uid="{DAB489D2-D8C2-4493-8DB9-D933617BCE4D}"/>
+    <hyperlink ref="A18" r:id="rId17" display="https://state.1keydata.com/kentucky.php" xr:uid="{BB8E9FEE-C1FC-436C-B81B-F99F3CF33F79}"/>
+    <hyperlink ref="A19" r:id="rId18" display="https://state.1keydata.com/louisiana.php" xr:uid="{47CD2271-F57A-4C93-8B8A-E175F9DC25D3}"/>
+    <hyperlink ref="A20" r:id="rId19" display="https://state.1keydata.com/maine.php" xr:uid="{696FE484-AF5D-4275-BEAC-CA2A9B91E306}"/>
+    <hyperlink ref="A21" r:id="rId20" display="https://state.1keydata.com/maryland.php" xr:uid="{848C9F60-1B78-4728-B3B2-11F5FDBAF18B}"/>
+    <hyperlink ref="A22" r:id="rId21" display="https://state.1keydata.com/massachusetts.php" xr:uid="{65685229-3E48-4624-A514-AF998DC09814}"/>
+    <hyperlink ref="A23" r:id="rId22" display="https://state.1keydata.com/michigan.php" xr:uid="{3B6313F6-0A70-4F36-9A3F-A6F2D667817B}"/>
+    <hyperlink ref="A24" r:id="rId23" display="https://state.1keydata.com/minnesota.php" xr:uid="{53C2CC79-9C37-4E14-902D-2F1EBB3DC32D}"/>
+    <hyperlink ref="A25" r:id="rId24" display="https://state.1keydata.com/mississippi.php" xr:uid="{D243D5F7-C97C-4A86-9948-94AF122BD89E}"/>
+    <hyperlink ref="A26" r:id="rId25" display="https://state.1keydata.com/missouri.php" xr:uid="{A2801156-5393-4FF3-ACB5-DC74A4936F00}"/>
+    <hyperlink ref="A27" r:id="rId26" display="https://state.1keydata.com/montana.php" xr:uid="{4DDD9FB0-3AB6-47BE-84CA-33056B28C7F7}"/>
+    <hyperlink ref="A28" r:id="rId27" display="https://state.1keydata.com/nebraska.php" xr:uid="{B2ED209B-EFB1-492A-9277-E442426CBD4D}"/>
+    <hyperlink ref="A29" r:id="rId28" display="https://state.1keydata.com/nevada.php" xr:uid="{C2B6E048-65E5-41D0-871D-151EC25EAFA9}"/>
+    <hyperlink ref="A30" r:id="rId29" display="https://state.1keydata.com/new-hampshire.php" xr:uid="{F3577E82-C6D7-4532-86BB-325E0F092D04}"/>
+    <hyperlink ref="A31" r:id="rId30" display="https://state.1keydata.com/new-jersey.php" xr:uid="{C5BE69F9-14E0-4D01-B38D-14E74273A248}"/>
+    <hyperlink ref="A32" r:id="rId31" display="https://state.1keydata.com/new-mexico.php" xr:uid="{C74BEB2A-EDCF-4AAB-8B12-25FF38DDFC30}"/>
+    <hyperlink ref="A33" r:id="rId32" display="https://state.1keydata.com/new-york.php" xr:uid="{DAA1D700-972B-4EA1-99C3-2C843EADE48B}"/>
+    <hyperlink ref="A34" r:id="rId33" display="https://state.1keydata.com/north-carolina.php" xr:uid="{90E79B03-7106-4FF1-A746-14D3D3A39497}"/>
+    <hyperlink ref="A35" r:id="rId34" display="https://state.1keydata.com/north-dakota.php" xr:uid="{A5D2581E-1FBD-4DF9-A15D-F570D6B09EDF}"/>
+    <hyperlink ref="A36" r:id="rId35" display="https://state.1keydata.com/ohio.php" xr:uid="{A9AFF7C4-41AB-4BAA-AE07-DC79AD68A17C}"/>
+    <hyperlink ref="A37" r:id="rId36" display="https://state.1keydata.com/oklahoma.php" xr:uid="{9405CCC4-606C-4856-ABE2-83B3F72F2186}"/>
+    <hyperlink ref="A38" r:id="rId37" display="https://state.1keydata.com/oregon.php" xr:uid="{9FB3B5AA-5334-4D12-90CD-130D956D6152}"/>
+    <hyperlink ref="A39" r:id="rId38" display="https://state.1keydata.com/pennsylvania.php" xr:uid="{52D4C6A8-D8D9-4096-B2B9-E55A2F3388E9}"/>
+    <hyperlink ref="A40" r:id="rId39" display="https://state.1keydata.com/rhode-island.php" xr:uid="{F0D395DD-C6D5-434F-AE51-AC19A46BB531}"/>
+    <hyperlink ref="A41" r:id="rId40" display="https://state.1keydata.com/south-carolina.php" xr:uid="{2EC88C7B-5678-4EC6-999E-00BF03F0A65B}"/>
+    <hyperlink ref="A42" r:id="rId41" display="https://state.1keydata.com/south-dakota.php" xr:uid="{F45830B5-E60D-4FE0-8498-E5EA018ADC4B}"/>
+    <hyperlink ref="A43" r:id="rId42" display="https://state.1keydata.com/tennessee.php" xr:uid="{3159AE8B-C86C-4D42-B8CA-81CD3040D913}"/>
+    <hyperlink ref="A44" r:id="rId43" display="https://state.1keydata.com/texas.php" xr:uid="{C644E441-99E1-43C3-AD93-46046DB2B920}"/>
+    <hyperlink ref="A45" r:id="rId44" display="https://state.1keydata.com/utah.php" xr:uid="{7951D014-7331-43DF-9227-6810FEF48140}"/>
+    <hyperlink ref="A46" r:id="rId45" display="https://state.1keydata.com/vermont.php" xr:uid="{F65F39C8-5EEB-47BC-927C-A71E472CE1CD}"/>
+    <hyperlink ref="A47" r:id="rId46" display="https://state.1keydata.com/virginia.php" xr:uid="{137664BF-CFED-4997-9C7B-B7CF5E84F63D}"/>
+    <hyperlink ref="A48" r:id="rId47" display="https://state.1keydata.com/washington.php" xr:uid="{270E5710-6AAF-409B-9993-F717B633AEB6}"/>
+    <hyperlink ref="A49" r:id="rId48" display="https://state.1keydata.com/west-virginia.php" xr:uid="{E1781213-0A6E-4777-ABEB-4EC3D1727395}"/>
+    <hyperlink ref="A50" r:id="rId49" display="https://state.1keydata.com/wisconsin.php" xr:uid="{E794A894-3E0F-41FA-9217-DB360B278E19}"/>
+    <hyperlink ref="A51" r:id="rId50" display="https://state.1keydata.com/wyoming.php" xr:uid="{9B0DB648-20AF-446A-BBDE-351804DAA998}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId51"/>
 </worksheet>
 </file>
 

</xml_diff>